<commit_message>
updated path to resolve issues
</commit_message>
<xml_diff>
--- a/output/report_category_per_gender_20220406.xlsx
+++ b/output/report_category_per_gender_20220406.xlsx
@@ -136,220 +136,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'Report'!B5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Report'!$A$6:$G$7</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Report'!$B$6:$B$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'Report'!C5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Report'!$A$6:$G$7</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Report'!$C$6:$C$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>'Report'!D5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Report'!$A$6:$G$7</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Report'!$D$6:$D$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <strRef>
-              <f>'Report'!E5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Report'!$A$6:$G$7</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Report'!$E$6:$E$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <strRef>
-              <f>'Report'!F5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Report'!$A$6:$G$7</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Report'!$F$6:$F$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <strRef>
-              <f>'Report'!G5</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Report'!$A$6:$G$7</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Report'!$G$6:$G$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>19</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -634,7 +420,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -736,6 +522,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>